<commit_message>
Fixes business scraper bug and adds new review files
</commit_message>
<xml_diff>
--- a/data_annotation/output_to_annonate/file_0_dimitra.xlsx
+++ b/data_annotation/output_to_annonate/file_0_dimitra.xlsx
@@ -469,12 +469,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Mr Captain Giorgos was exceptionaly friendly, welcoming and nice .  I lived an unforgetable experience in the blue aegean sea and I would undoubtably recommend it to everyone !!</t>
+          <t>My girlfriend and I went on the fishing trip with Tina and her father and it was the most wonderful day of our vacation. We went along the south shore of Milos and the views were breathtaking. We did snorkling in otherwise unaccessible locations, we fished the coast and we stopped in Kleftiko to have lunch with expertly cooked, freshly caught fish. Tina and her father are great cooks, the food was unbelievable. Please, do not skip on this incredible, almost private experience. I will never forget it!</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Unique Experience</t>
+          <t>Unforgettable day with the nicest hosts!</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
@@ -485,12 +485,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Just go...  Captain Anthi &amp; Crew are super-nice.  Lots of fresh fish to catch &amp; EAT. (From cages (for shrimps &amp; octopus) &amp; 1km-long net PLUS you can fish yourself.)  Fresh shrimps (caught in hand-made cages by Anthi's father)... super-big octopus.  Time well spent. ***  PS:…</t>
+          <t>We had a fantastic day on the sea with Antonia and Michalis and their wonderful daughter Nikki who entertained our young children. Coffee and cake in the morning followed by a delicious homemade lunch right on the boat! Swimming in the crystal clear waters was an extra special treat!! Definitely recommend this trip to experience an authentic day on the sea with a great Greek family!!</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>FANTASTIC! *****</t>
+          <t>Awesome Day on the Sea!</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -501,12 +501,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>By far this was my favorite memory of my visit to  Santorini. Anthi, our Captain, she is simple the best! She is passionate, she is knowledgeable, polite, friendly and treat you like family. Girl Power! Marcos and Muhammed the other members of this amazing crew complete the…</t>
+          <t xml:space="preserve">We spent the day with Effy, Dimitrios, Mohammed and Eva on the 1st Aug to celebrate my dad's 70th,  superb day had by all,  the team attended to our every need, so friendly, my 10 year old son got involved in assisting with the mornings fish catch,  hauled in red mullet, barracuda,scorpion fish, several squid the list went on and in. Moored up on beautiful remote beach, whilst snorkeling we were cooked a superb meal by the talented Effy,  delicious food all round,  tasted lobster, along with home grown vegetables, wonderful day, our group did not want it to end and Effy and Dimitrios truly had a great day with us also.  Cannot recommend this trip enough, they will do their upmost to accommodate any special requests your group may have I'm sure.  So friendly and a definite trip we will not forget. My dad had a day he said he'll never forget.  Thank-you to all your team and hope to see you again one day! </t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>A magnificent tour!</t>
+          <t xml:space="preserve">Brilliant Day Out! </t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -517,12 +517,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Best fishing trip ever! My 13 yr old son wanted to go fishing and we contacted Giorgaros fishing trip with our hotel Consierge.  They were amazing and very professional a true family experience.  My son loves to learn about the different fish in the area and we caught an amazing…</t>
+          <t>Snorkel in turquoise waters, bring in multiple catches, and chat with Giannis who has been fishing half his life!  Not only charismatic and friendly, this young man is tireless and skillful.  His innovative luring method ensures everyone will enjoy the sensation of a fish on the line.  Line caught on the boat?  Giannis will dive underneath and free it. Interested in spearfishing?  Watch Giannis dive amazing depths and bring up a grouper.  Afterwards he'll prepare your catch on the boat along with tasty sides, wine, beer and homemade lemonade.  Don't miss a day on the water in the most comfortable boat around for the most reasonable price available with the most competent, knowledgeable captain we've met.  Just fabulous!</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Fishing trip in Santorini</t>
+          <t>Captain Giannis is the best!</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
@@ -533,12 +533,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>It is my first time ocean fishing.Giorgos is the best captain! He is knowledgable, and likes to share with people.  Such a good experience. It's not only about fishing. The food we got is fabulous as well!!</t>
+          <t>We had really fantastic time with this tour. We were ten people and it felt like having a private boat to ourselves to enjoy. The captain and the daughter are really nice people and the fishing part was good fun. The lunch , the fresh fished cooked on the boat, was amazing,plus there were many more thing to eat, from the cake in the morning to some snack before lunch and plenty of drinks. I appreciated a lot that the swimming stops were very long without any stricht time schedule and in spots that were a bit aside from where the other bigger boats. From what I have seen around, I believe this trip offers you something different from the other tours and it is really worth it particularly if you are more interested to enjoy a day on the sea more than making the tour of the entire island.</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Fantastic day with Giorgos</t>
+          <t>Fantastic Day</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -549,12 +549,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>First I just wanted to try the fishing experience in Skiatos.I chose Dimitris's fishing boat and it was the best choice I have ever made! I went fishing for about 4 hours and we had everything at our disposal: a complete fishing equipement, sandwiches, beer, water, fruits,etc.He…</t>
+          <t>Not much to say about this day except... Absolutely perfect!!! The entire boat was for us and hosted by this beautiful couple that gave us the complete experience of what we were looking for.Nikos the captain knows everything about those islands and where to go to make you spend a perfect day for fishing, discovering nice spots for swimming and show you some breathtaking places ; can’t forget about madame also, Frosso who’s a really good chef and knows how to host you perfectly.Well, if you pass by Milos don’t hesitate go to this place you won’t be disappointed that’s for sure.</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Excelent fishing and sailing experience</t>
+          <t>What a day!!!</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
@@ -565,12 +565,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>I had the opportunity to learn a lot about fishing tradition. I had a wonderful time as the boat is cosy and the crew is very responsible and experienced!!!</t>
+          <t>It is my first time ocean fishing.Giorgos is the best captain! He is knowledgable, and likes to share with people.  Such a good experience. It's not only about fishing. The food we got is fabulous as well!!</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>A perfect fishing trip!</t>
+          <t>Fantastic day with Giorgos</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -581,12 +581,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>This was such a special day out for us with Giannis and Nancy and their lovely daughter on their fab fishing boat. Just a nice small group of us spent the day out in the water - they were so friendly and helpful - we all caught fish including our 11 year old son who was so…</t>
+          <t>So my boyfriend was keen to go on a fishing trip and was absolutely buzzing about this trip. I originally was not so much....but I took a sea sickness tablet and thought I’d give it a go! We first set sail and it was a bit rocky but it was okay! I was such a novice and struggled to catch anything at first but I caught one fish, so I was happy! My boyfriend and all the other members of the boat were catching loads, including puffer fish (which you cant eat but are nice to see!) it was so calm sat on the sea under the shaded canopy.The team were always around to give you any tips to help you! After some time fishing we stopped off for snorkelling while the team cooked up what we had caught. This was my highlight of the trip. Sitting looking out to the sea eating bbq fish caught and cooked within a couple of hours was amazing. The crew threw bread into the water to attract the fish and they were all jumping out of the water. Beers and soft drinks were available and offered throughout. It was lovely sat at the front of the boat with a cold beer staring out into the sea!My boyfriend came away saying it was definitely his highlight and I’ve got to say I would definitely do it again too! Thanks to the whole team! We even recommended you guys to a couple back at the hotel!</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>The best day of our holiday by miles!</t>
+          <t>Never fished before but this was so good!</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
@@ -597,12 +597,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>We have had a perfect day with cpt. Dimitris. He offered us good price &amp; delivered good service. We visited Lalaria and Castro beach had a lunch there in taverna and on the way back stopped for a quick fisiing. Relaxed atmosphere, music &amp; beer - we will do this again!</t>
+          <t>We were 3 friends we had a lovely time with vassili he was upset nice and careful You shouldn’t miss it if you’re in Rhodes!!!!</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>What a day on boat !</t>
+          <t>Amazing!!!!!</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -613,12 +613,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2nd review as 1st one lost! My husband and 2 friends had the pleasure of going on this trip on Mon 3rd Sept. Antonia and Michalis were fabulous hosts from the moment we stepped on board and I hold a lot of memories from this day. We had a lot of laughs with the other guests and…</t>
+          <t>My husband and me book this tour it was a really nice trip the tourgides was friendly we feel home from the first moment .We have a perfect meal swim and sunset .We will come back...go on like this .Best regards‍️</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>a truly unforgettable day</t>
+          <t xml:space="preserve">Perfect </t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
@@ -629,12 +629,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>I spent two weeks in Kos and I booked a fishing trip before the arrival, via facebook.  I enjoyed it so much, the price was good for a 4 hour trip and we caught great fish so I rebooked a second trip with captain tasos! We liked that we took the fish and a restaurant in the…</t>
+          <t>We did this cruise a couple of days ago. All I can say is amazing! You start the cruise by collecting the fish net (actually cpt Andreas does it). Afterwards we went to the beautiful and almost “private” beaches of Poliaigos island which are really the highlight of the area in my opinion. We stopped at an amazing beach ,all by ourselves , to swim and afterwards have our lunch: the fresh fish we just cought ( “kakavia” a tradiftional Greek soup made of fish) and tasty home made “ladenia” - a traditional kind of pizza in Cyclades-by the captains mom. This was accompanied by salad made of tomatoes cucumbers and green peppers grown by the captains dad in milos! A really special and original meal! We stopped at several beaches of Poliaigos which are extremely beautiful and have the clearest water, astonishing landscape and all kinds of colors!At our final stop at pano Mersini beach we had home grown melon after our swim so that we would have the strength to “help” the captain throw his fishing net again in the sea :-) .Andreas the captain and his helper Andreas , made this experience so special and unique! One of the must do of milos and Kimolos! I highly recommend this!</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Fishing</t>
+          <t>A unique experience! MUST do it!</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
@@ -645,12 +645,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>This fishing trip was one of my favorite experiences in Santorini! It was very authentic and I felt immersed in the Greek fishing culture. Our captain was very interactive and explained each fish/sea creature we caught. She has an incredible and impressive life story. The meal…</t>
+          <t>Great experience!!!  Getting fish out of the nets is such a fun! The greek flair at sea. Captain George - a higly skilled sailor, his mother in law -the best cook ever- and Sadik will make your day. Dont miss it.</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Fishing Excursion</t>
+          <t>A joyful day at sea</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
@@ -661,12 +661,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Went with these guys in the evening for a leisurely fishing trip.  Great time. Focused on quantity rather than size at our request and did not fail to deliver  Nice food &amp; drinks included at competitive rates  Thank you and hope to see you when we return</t>
+          <t>Well, what can I say, came with 13 mates, booked with George a while back, and we had a brilliant day!!  Great fun, swimming, great hosts, and the lunch/ wine etc was lovely! Caught some fish too, and had a swim with a turtle! Great thanks to George, his mum in law, and other crew, a great day!</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Brilliant time</t>
+          <t>Sniffer’s 50th!</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
@@ -677,12 +677,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Amazing experience on a Truly authentic, family run Greek fishing boat.  Fantastic to see all the different varieties of fish being reeled in, including my favourite - Lobster -  Lots and lots of Lobsters - I have never eaten so much Lobster in one meal! Absolutely delicious! …</t>
+          <t>When not taking you on a trip around the island with his daughter Ntina, Kyriakos is a fisherman. This trip is the perfect mix between a touristic hop between the unaccessible beaches of Mílos, the experiencing or Paragadi fishing, and the tasting of traditional fish soup (fresher fish, you die! You’ve just taken it out of the water!)Avoid the big boats. You’ll just spend the day with 30 to 50 other tourists. Let Kyriakos and Ntina share a bit of their daily lives.These guys are a bit hard to find, so look for them in the port of Adamantas! The boat is called Anna Maria (Kyriako’s granddaughter).</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Best trip ever in all my world travels.</t>
+          <t>Ever felt at home on a boat?</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
@@ -693,12 +693,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>What a great day out with Dimitrios and Efi, they were such warm hosts, and couldn't do enough for us. It was really interesting and fun to see the catch brought in, and help the fisherman. Then while the catch was being prepared we visited private beaches, and even had a clay…</t>
+          <t>Captain Kyriakos is an authentic man and very joyful person and his daughter Tina was very kind.They are both very friendly and full of humor!! We went for fishing and caught many fishes!! Mr Kyriakos and his daughter Tina cooked the fishes and other tradiniotal greek dishes. They also provided delicious breakfast and fruits! The trip and the beaches we visited were amazing (Gerakas, Tsigkardo, Kleftiko) . The fishing trip is for maximum 10 persons therefore i suggest to book 2-3 days before. The most amazing and authentic experience!! Thank you so much Captain and Tina!</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Great day out!</t>
+          <t xml:space="preserve">Amazing and Authentic Experience </t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
@@ -709,12 +709,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Amazing day with 2 of the nicest people you'll meet! Beautiful swimming locations and everybody will catch fish!</t>
+          <t xml:space="preserve">A fabulous day out fishing with Dimitris on his own boat. We caught 98 fish between 7 people which was excellent and was shared out at the end of the trip. Needless to say we had to give it to one of the tavernas in return for a very cheap dinner. This is a great day out for anybody, couples and families alike.Stopping off for a swim and also lunch. I would love to do it again on another visit to Skiathos </t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>One of the best days on the island</t>
+          <t xml:space="preserve">The Best day out </t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
@@ -725,12 +725,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Not really sure what to expect and having to be at the boat at 7.30am was not the holiday experience I was hoping for. However from reaching the beach and being greeted by a beautiful sunrise to meeting Efi, Dimitrios and his parents on the boat my concerns had disappeared. The…</t>
+          <t>amazing people!we catches a lot of fishes!we drunk greek tsipouro and we grilled the fishes we catched</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Unique</t>
+          <t>fishing</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
@@ -741,12 +741,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>I did the Fishing experience with friends and family a few days ago. Mr Nikos and his wife are very friendly and know all the good spots and beaches! Mr Nikos picked us up from Kimolos at exactly the agreed time, we went and gathered the nets, and then went to a number of…</t>
+          <t>Antonia and her husband are the most wonderful, heart warming and lovely people you can spend a day on the boat with. We were shown how the fisherman is working daily - collecting the nets , checking the fish and later on throwing it back again in the sea to collect it the next day again!!!! And the best of all , you get to eat the most freshest and delicious fish of your life( for me especially , as I life in a big city far away from the sea).  Antonia is a fantastic cook , so she made sure we were all happy the whole day provided with lots of deliciousness!!! And the whole group was so nice to spend with, getting to know so many different life stories, having a break from your rational brain, relaxing your mind and feeding the soul!!! Thank you Antonia and Michaelis.... you Are the best!!!!</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>A must do experience</t>
+          <t>Beautiful sail away :)</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
@@ -757,12 +757,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>From the very start of our day out until we left our hosts in the early afternoon, this was just a fantastic experience. We tried our hands at fishing ( harder than it looks!), steering the boat and just enjoying being on board with such hospitable and friendly hosts. Nothing…</t>
+          <t xml:space="preserve">Went on this fishing trip with my sons - 16, 14 and 8. This was a lovely quiet trip with just a small boat and a small group of people. Run by such friendly people. We had a great time fishing, had the chance to swim between stops and were served a great lunch with fresh fresh sea bream. Highly recommend this trip - you will find their stall on Mandrake Harbour at the end nearest the deer statues. </t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>The Best Day of our holiday</t>
+          <t>Best day of our whole holiday</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
@@ -773,12 +773,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>We had a great time. The captain was nice. We caught some fish. Had a nice meal on the boat. Awesome!</t>
+          <t>A great and authentic experience ! We had a very nice day. Many thanks to Tina and her father for all they shared with us. You are so kind people. A real human experience Thank you for the excellent lunch !See you next time in Milos.Efharisto poli</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Great experience!</t>
+          <t>A memorable day</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
@@ -789,12 +789,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>I had a great day today, Anthi was warm from the first email to the goodbye hug.   Anthi is passionate about fishing, the marine environment and conserving it and knows the local area like the back of her hand. She and her crew are great accompaniments with a huge diversity of…</t>
+          <t>We go with Nikos, his wife Froso and Simon to the FishingTrip it was great ... best food fresh from the Ocean, very interesting to see the work of fishermen, speaking about living on milos and the traditions ... beautiful places for swimming! and looking!!! Snacks, fishsoup, baked fishes, greek  coffee, yoghurt with homemade sweets and watermelone, Drinks how much we want and a Ouzo before  leaving the boat!!! A very nice and  perfect day! Thanks so much Anita and Bernd.... a „must to do“ staying in Milos</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Fantastic trip with passionate, sustainable local family run business.</t>
+          <t>Perfect day</t>
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
@@ -805,12 +805,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Me and my family had a great time with Antonis and Villy! We went for fishing we had very joy and it was lovely experience! We laughed and really fulled our batteries!! Surely recommend them!!!</t>
+          <t>We had a fantastic time with crew and another couple, nearly a private tour!. We had fab food, crystal clear and calm waters for snorkelling, a fab fishing experience, catching all types of fish and octopus.. we will definitely do it again with the kids next time.. if you fancy a boat trip i would recommend this above anything else.</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Amazing experience!</t>
+          <t>Best part of the holiday</t>
         </is>
       </c>
       <c r="C23" t="inlineStr"/>
@@ -821,12 +821,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>We now live in Zakynthos and this trip was recommended to us by friends they raved about it so much we booked and took along our daughter and her partner, leaving from the Port of Zakynthos we headed out to sea, George (Captain) explained what we would do and what we would see…</t>
+          <t>This trip was booked to celebrate a birthday, there were 7 of us in our group and it was the most amazing day ever.  I was a little worried about sea sickness which I had suffered from before, I have to say I didn’t, feel unwell at all.  The whole day from start to finish was excellent, Giorglas and his crew where most welcoming and informative the whole day,  from putting the nets out to  the surrounding area and the bays we stopped in.  The food was delicious,  and we enjoyed sitting and chatting with the Other 5 guests on board.   Yes it was an early start but so worth it</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>If you do one trip in Zante - do this one!</t>
+          <t>Fantastic day Fishing</t>
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
@@ -837,12 +837,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Firstly Dimitrios the owner and Captain of this boat is a super host and very kind and thoughtful with his guests. You couldn't want for a better fisherman to take you out. The boat is lovely and clean and not too big to be impersonal and not too small to feel cramped. We…</t>
+          <t xml:space="preserve">Had a fantastic afternoon on the water with captain Dimitris. Toured breathtaking islands near Skiathos, private beaches, to a special spot he knew about for urchins and fouscas (type of oyster) where he proceeded to dive, bring on deck and prepare a feast. HIGHLY recommend! He was professional and easy going the entire journey and had everything to make the trip special including music, cold beer and a fresh fruit platter he made up on the spot. Will remember always  </t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Wonderful day with my son fishing</t>
+          <t xml:space="preserve">Blissful afternoon !! </t>
         </is>
       </c>
       <c r="C25" t="inlineStr"/>
@@ -853,12 +853,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>What an amazing day i had yesterday with this lovely couple Giannis and Nansy.  So good organized, beautiful and delicious food, super cold drinks, we had a fantastic group of people and you visit the most beautiful bay's of Samos. I will make the trip again.</t>
+          <t xml:space="preserve">Hello from the Norwegians.My fiancé Sam and I booked this boat trip as our wedding present to one of our favourite friends :) We wanted to book a whole day trip with authentic Greeks and authentic Greek foods and views. And that is exactly what we got!Antonia, Michalis the boat captain were absolutely amazing hosts and company throughout the whole trip! The trip started with the crew picking up the nets of fish. After that the boat travelled quite a distance to get to a quiet location near a beautiful beach with cliffs and a gorgeous view. We got to swim for a long time around the beach and boat, and the water was so warm and delightful. Then we were served beautiful starters (Greek style bruschetta), and after a while we were served a full main meal consisting of lobster, fish, spaghetti, Greek salad, Greek potato mash and beautiful local white wine. Throughout the whole trip the crew made sure we were informed of all the sights and fun local facts about the island. The crew were really good with mingling with us, but also give us some space to eat and space when needed.The married couple could not have been happier and more pleased with the gift, and kept saying throughout the entire trip how amazing the trip was!We could not have been more thankful, amazed and grateful for the trip, and want to thank the crew once again!We definitely recommend this trip highly! One of the most amazing things to do when visiting Kefalonia All the best and greetings from Norway,Karoline, Sam, Marita and Gunnar </t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Fantastic and amazing fishing trip</t>
+          <t>An authentic and amazing Greek boat trip 🇬🇷</t>
         </is>
       </c>
       <c r="C26" t="inlineStr"/>
@@ -869,12 +869,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>My family and I joined captain Kyriakos and his daughter to a fishing trip in the south of Milos island two days ago. This was an excellent experience that we have enjoyed very much. With  a small team of another 7 people (12 in total) we have visited some of the most beautiful…</t>
+          <t>This was a wonderful experience for my husband and I and our two boys, ages 8 and 10. KNOW this is traditional fishing with nets, pots and SMALLER fish. One of the people on our boat expected deep sea sports fishing and was disappointed. If you want that, and catching big fish, Giorgaros does private outings or this but you need to specify that. We were very happy to have great hosts, great food, beautiful scenery, pull up shrip, fish etc and enjoyed it immensely! Just know that if you want BIG fish, you need a private charter with them and book appropriately.</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Fishing trip in Milos island</t>
+          <t>LOVED IT! BUT know what to expect</t>
         </is>
       </c>
       <c r="C27" t="inlineStr"/>
@@ -885,12 +885,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Anthi brings you to a moment out of time. Far from all the sterelised cruises proposed on the island, you will live an amazing experience. Helped with An amazing team, she is going to show you the traditional way of fishing in Santorini (with the traps and the nets). Then you…</t>
+          <t>Thank you for a fabulous day on the sea with your family.  We had a great day, were well looked after and enjoyed the delicious food that kept coming all day.  Next time we will catch  that big fish!!!</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Just a wonderfull time! 🔵⚪️</t>
+          <t>Fabulous day on the sea</t>
         </is>
       </c>
       <c r="C28" t="inlineStr"/>
@@ -901,12 +901,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>This is a must if you visit Rhodos. An amazing experience with nice fishing and swimming. And then to top It all of,  we got a good meal with grilled Fish, greek sallad, bread and beverege. And a slice of watermelon to end a  Nice meal 😋  Very Nice staff and Captain. We highly…</t>
+          <t>My wife, daughter, and I went on the sunset fishing tour and we had an absolutely wonderful time.    Captain Anthi is a fantastic host and she did such a great job telling us about Santorini and its beaches as well as teaching us about the traditional fishing methods on the island.   They then put on a one of a kind dinner in which we were constantly be served by her and her crew.   If you have time while you are in Santorini I highly recommend you take her tour and enjoy a great experience, a great crew, and a beautiful sunset.</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>An amazing trip  🎣</t>
+          <t>An amazing trip with a spectacular crew.</t>
         </is>
       </c>
       <c r="C29" t="inlineStr"/>
@@ -917,12 +917,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>A great fantastic day fishing, lovely people, fabulous food, great no matter what age this family run business are kind friendly and have a great sense of humour, nothing is to much trouble, it is also very educational.Have already booked for a second trip. A big thank you to…</t>
+          <t xml:space="preserve">From start to finish the day couldn't have been more perfect ! We were welcomed onto the boat by Efi  and Demetrios as if we were old friends and by the end of the day we certainly felt as if we had known them longer than a day. Efi and Demetrios along with Mohammed and Demetrios parent's made the day so wonderfully special. The hauling in of the fishing nets.. to us novices trying to get our catch (lunch )of Red snapper .. Sea bream ... Squid .. out of the nets ... very very  tricky but made to look so easy by Efi who I hasten to add had the patience of a saint with us when we seemed to get the fish more tangled up in the net's !!! We had 2 opportunities to cool off in the sea. Once in the morning we swam in the clearest blue water onto a little cove to dry off before swimming back to the boat for refreshments and again before lunch we anchored at another stunning cove where Demetrios Mum showed us how to use the clay from the beach to have a clay body scrub ... Just fabulous ! Lunch was cooked and served by Efi on the boat . The fish caught in the morning was cooked to perfection  the organic vegetables and salad all from Efi and Demetrios garden just delicious !! The wine served was another product of Efi and Demetrios making !! The day was definitely the most memorable of our holiday and one that when we return to Katelios we will do again !The only disappointing thing about this trip was that it ended too quickly and that Jame's (a fellow day tripper ) didn't catch any fish with his rod he had bought all the way from Scotland .. But at least Demetrios Dad got the use of the rod whilst we were swimming and the amazing man did catch a fish !!! Unique trip with great company. Thank you Efi, Demetrios , Demetrio's lovely parents and Mohammed !! </t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t xml:space="preserve">An amazing day out well worthwhile </t>
+          <t>Perfect !</t>
         </is>
       </c>
       <c r="C30" t="inlineStr"/>
@@ -933,12 +933,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>We have just been on our third trip with Antonia &amp; Mixalis and it was as excellent as ever. Once on board the boat you are offered coffee and cake to start off your day. You then sail to where the nets have been set the previous night and the catch is pulled in onto the ship.…</t>
+          <t xml:space="preserve">A relaxing day with great people and a real taste of Greece. Fishing on the boat, releasing the fish from the nets and then our captain cooked the catch for us whilst we lay on a secluded beach! Turtles and a bit of snorkelling too.  The food was amazing, fresh &amp; tasty.  Nothing too much trouble.  You have to try this, more personal, very traditional and we learnt something too.  Thank you Maria and Captain - we loved it! </t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Another excellent trip</t>
+          <t>A taste of Greece</t>
         </is>
       </c>
       <c r="C31" t="inlineStr"/>
@@ -949,12 +949,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>This amazing family gave us the possibility to experience a unforgettable day full of emotions, happiness and amazing traditional Greek food. This trip included everything starting from fishing your own food over seeing the most amazing places of santorini, taking a bath in…</t>
+          <t>The fishing experience was enriching and one-of-a-kind, and the crew members friendly and thoughtful (not to mention incredible cooks). We watched them fish, name, and clean all kinds of fish (we even caught an octopus!) and observed other kinds of marine life at the same time. The route taken was varied and interesting, with some stunning waters, beaches, and volcanic rocks.This fishing tour is for people who enjoy eating fish, love the ocean water and want a truly Greek experience (and who want to taste the best fish broth they've ever had).If someone has issues with fish bones, we would recommend they call in advance and let them know, so they can serve and prepare additional food, which is what they did for us, as they are very accomodating and kind.Thank you Andreas, Andreas and Marios!</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>The trip of the dreams</t>
+          <t>Very friendly people, excellent fresh fish and great experience!</t>
         </is>
       </c>
       <c r="C32" t="inlineStr"/>
@@ -965,12 +965,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Had an unbelievable day out in the crystal clear waters surrounding Poros with our captain Giannis. We watched as he spear fished two Parrot fish for our lunch as we snorkeled at beautiful protected spots along the coast. As 6 friends in their late 20s this was the perfect day…</t>
+          <t>Travelling as a family, generally its difficult to find activities a couple and Girls would be happy to do. despite early reservations (would girls be ok with the fishing) we embarked on our trip and had a most wonderful experience.Captain Vassilli and his co pilot Mark were excellent and basically taught us all to fish, They showed great patience and skill with our 10 year old who initially found the sport alien, however she went on to catch 5 good fish...  and thoroughly enjoyed her day. to a man we all agreed this was a holiday highlight. Food was fabulous and included some of our catch... well done Makarounas Fishing Trip. Highly recommended.</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Snorkeling and fishing bliss</t>
+          <t>The best family fun we had in Rhodes..........</t>
         </is>
       </c>
       <c r="C33" t="inlineStr"/>
@@ -981,12 +981,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Fantastic experience - great views as you leave the city and then some brilliant fun fishing for a couple of hours. Quick swim around the caves and hop back out for you bbq’d fish for lunch/dinner. Great fun and trying to persuade my other half to do a second trip in the same…</t>
+          <t>we had agreat time at dimitris boat. the man is amazing he duved and brought up axinous and petalides as they are called at their islands. so kind and great host ,</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Brilliant experience - definitely worth time and money</t>
+          <t>fishing trip amazing</t>
         </is>
       </c>
       <c r="C34" t="inlineStr"/>
@@ -997,12 +997,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>An experience I would highly recommend!Yiannis was an amazing host and the fish turned out delicious.</t>
+          <t xml:space="preserve">Antonia is a delicious person, so kind and so sweet: she came to peek us up early in the morning because we were a little bit far from the port! The day started with an amazing slice of cake cooked by herself and continued with a lot of great food and mostly important with a lot of fun! The company was great, we enjoyed the day so much from the first minute to the last.The beach we saw was incredible, we dived and swam all day. And lastly, I’m Italian and I can tell that the spaghetti that Michaelis and Antonia Made were simply PERFECT. Most beautiful day in Cefalonia.Thank you thank you thank you! </t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Everything was amazing!</t>
+          <t>Best experience ever!!</t>
         </is>
       </c>
       <c r="C35" t="inlineStr"/>
@@ -1013,12 +1013,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>We had such a great time during our excursion together with Niko and his Wife and their team! Very intimate boat trip (10 people), great fresh and tasty food (0km fish - we ate all fish fished by the boat fisher during the morning!), wonderful blue crystal water and last but not…</t>
+          <t>One of the highlights of our trip.  Where else can you go fishing and the captain prepares your catch for your while you swim?  The lunch setup is super cute where they have your cooked fish, salad, and a side of bread for you all prepared for you at the "table" so when you hop back on the boat after your swim, all you do is eat.  With the food scraps you throw them into the water and a bunch of fish will fight over it.  It was fun watching that.  The fishing we caught that day were all very tiny though, so don't expect any big catch?  I'd def. recommend this fun half day trip with Makarounas if you are sick of lounging at the beach.</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Amanzing fishing boat trip in Poliegos!</t>
+          <t>Free drinks and fresh lunch prepared for you</t>
         </is>
       </c>
       <c r="C36" t="inlineStr"/>
@@ -1029,12 +1029,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Really relaxed and friendly fishing trip along the coast of Rhodes with our two teenage daughters.  The captain and his son (I think) were super friendly and couldn't do more for you.  The fishing was fun but the highlight was jumping off the boat for a swim and the delicious…</t>
+          <t xml:space="preserve">I feel I have to be honest on my review and looking at the previous 5* reviews unfortunately I don’t agree. Firstly it was great to be aboard a fishing boat seeing how the nets work and then to see the catch of day. Coming from a farmers background this was something we were interested in - seeing where our food came from. We caught lots of lobster and I believe ray. The food on board was lovely and freshly prepared. However we felt that we had to eat the lobster, this was caught that morning on the boat however me and my partner had no intention of eating the lobster. (I know some people may think we were being fussy but this is the only food we’re not keen on - were also weren’t the only ones) and would have declined knowing that all the lobster was being cooked. We would have tried but felt pressured into all the lobster being eaten which then pushed us further into saying no thank you. We enjoyed the bruschetta (best I’ve ever had) and the spaghetti and soup. There is a lot of food provided. Also we did stop for a little swim while lunch was being prepared however just be aware that the boat doesn’t stop on a beach as mentioned in our itinerary. Instead stopping near cliffs. If you not keen on deep water (me) then a life jacket is provided. However I know some people prefer to wade in the water and feel that this is important for people to know. My partner enjoyed his swim. We weren’t sure on rough timings so wasn’t too sure how long we had in the water - we had a long time (2+hours which was a little too long for us). Overall this is a lovely boat trip if you would like to see how the fishing world works. However for us we felt it was a little too long and at times felt we had done wrong by not eating the lobster. Perhaps state to the crew that this isn’t something you want to eat so they can accommodate you. It would have been nice to have been introduced to the crew too. It was nice to see a different part of the island and to be aboard a fishing boat eating freshly cooked food. </t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Fun, fishing and food</t>
+          <t xml:space="preserve">Good but could been better.... </t>
         </is>
       </c>
       <c r="C37" t="inlineStr"/>
@@ -1045,12 +1045,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>We wanted to get in some fishing while on Santorini. The typical “fishing charter” is not really available here, but we are so happy we found Athina, Marcos, and Mohammed! We had a great evening of food, fishing, and learning about the local fisheries. The food they prepared was…</t>
+          <t>This isan experience of a lifetime. We left zante Harbour while the sun was rising and then we stopped to put the fishing nets in the water then we had sone melon and drinks. Then we left the netd behind to go and have a swim at a beautiful secluded beach for a few hours. Then back to the nets to pull them back on board. A very successful catch too with a variety of fish caught including an octopus and a sponge. Then we sailed to another beach for a swim while the fish was prepared on board with wine spaghetti and bread. Absolutely beautiful meal. Giorgos the captain has a great sense of humour and lets you get involved in everything and if you're lucky he might let you stear the boat. Very clean and hygienic which i didn't expect. Couldn't recommend anymore, dont miss out!</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>A great way to mix it up from the typical catamaran</t>
+          <t>Fantastic trip</t>
         </is>
       </c>
       <c r="C38" t="inlineStr"/>
@@ -1061,12 +1061,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Great fishing, nice food and beautiful bay to swim. Small fish were annoying to catch. Got great beer to compensate that. 6/5</t>
+          <t>It was a amazing  trip with an astonishing view. The captain was friendly and willing to answer all of my questions. In all means it was perfect!</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Fishing Trip</t>
+          <t>A interesting boat trip.</t>
         </is>
       </c>
       <c r="C39" t="inlineStr"/>
@@ -1077,12 +1077,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>This fishing trip was definitely one of the best excursions I have ever been on and gave me a real insight into the hard work of a fisherman. As soon as you arrive are you greeted kindly by the crew and made to feel extremely welcome. You are provided with freshly made cake and…</t>
+          <t xml:space="preserve">We enjoyed a wonderful day with Anthi and her crew ( and her sister's gorgeous new born baby and beautiful little boy ) . She was such a lovely and kind person ( especially when I felt a bit sea sick ) and looked after us very well . Most of all though we loved to hear about her fishing family , how they live , what they do and feel her passion and pride . I loved the fact she was the captain !  We caught fish , swam in the sea and had a perfect meal of fresh fish on the boat . Met some other lovely people and had a very memorable day . Do this if you like the water and want to do something authentic . A great day . Thank you ! </t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Best trip ever!!</t>
+          <t xml:space="preserve">Great day ! </t>
         </is>
       </c>
       <c r="C40" t="inlineStr"/>
@@ -1093,12 +1093,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>What a day! We found this gem of a boat at the Adamantas port in Milos, after looking at many other options for a trip around the island and to the lovely beaches. Our initial impulse was to go on a sailboat- but they were fully booked. My husband and a friend found this little…</t>
+          <t>The highlight of our trip.  Our captain met our every desire.  Caught enough fish to feed an army.  The lunch was wonderful.  I would recommend this trip to everyone for the most delightful day on the sea you will ever experience.</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Authentic boat trip</t>
+          <t>Mrs</t>
         </is>
       </c>
       <c r="C41" t="inlineStr"/>
@@ -1109,12 +1109,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Alyki is a wonderful place in Paros for someone to visit! The ride by the boat of captain-Giorgis is a great and unique experience for me! Captain is very friendly and polite and he can take you to many nice sightseeings! If you go to Paros island don't miss this ride by boat !</t>
+          <t xml:space="preserve">I Had a really great time , if you can just try it !!!The captain is awesome !! Really friendly guy ! </t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>ride by boat with captain-Giorgis is a unique experience !</t>
+          <t>Suggested 100℅</t>
         </is>
       </c>
       <c r="C42" t="inlineStr"/>
@@ -1125,12 +1125,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Exceeded all expectations despite glowing reviews! Must, must do. Captain Anthi puts you on the bite. And her crew is competent and friendly. Just as all the reviews have stated earlier. That would be enough for a great day fishing. But these folks go way beyond. Anthi was…</t>
+          <t xml:space="preserve">My second time, my partner's first. Cannot recommend this experience enough. Remember it's not your ordinary excursion it's a a real fishing boat and that is what you are there to experience, which is what makes it so special. We both agree that we ate the best meal of our holiday on this boat.... Which considering the size of the kitchen is absolutely amazing. Antonia &amp; Mikalis thank so much </t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Authentic Aegean Fishing Trip</t>
+          <t>Wonderful Day</t>
         </is>
       </c>
       <c r="C43" t="inlineStr"/>
@@ -1141,12 +1141,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>We spent the day with Efi and Dimitrios celebrating our daughters 16th birthday and it was an amazing day that we will never forget. Efi and Dimitrios are wonderful, friendly people who make everyone feel really welcome. We started the trip with coffee and bread and Efi's…</t>
+          <t xml:space="preserve">Best fishing trip ever! My 13 yr old son wanted to go fishing and we contacted Giorgaros fishing trip with our hotel Consierge.  They were amazing and very professional a true family experience.  My son loves to learn about the different fish in the area and we caught an amazing variety in the local way.  Nets were set a day ahead and we harvested them the day of the trip, we caught lots of shrimp, cuddle fish, octopus and many fish varieties.  They fried some shrimp on the boat and provided lunch for us.  It does not get any fresher than that!!Big hurray for Giorgaros fishing tours for allowing us to join in their local fishing experience:) We will definitely come back. </t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>An unforgettable experience</t>
+          <t>Fishing trip in Santorini</t>
         </is>
       </c>
       <c r="C44" t="inlineStr"/>
@@ -1157,12 +1157,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>This fishing trip was the highlight of our holiday. Swimming, beautiful beaches, amazing scenery, fantastic lunch and wonderful hosts. Thank you both!</t>
+          <t>This was our second trip with Antonia &amp; Mixalis after enjoying our first trip so much.As it was early May the weather was unpredictable and our original trip had to be cancelled due to bad weather. However Antonia made sure we were re-booked in and had our trip. They will not travel if they think their customers will not enjoy the experience.We were provided with cheese pie and Greek coffee before we set sail at 8am.We set sail to the nets that were laid the previous night and then watched as they landed a great variety of sea life.Once the nets were hauled in we sailed to a beautiful secluded area where we stopped for a relax and if brave enough a swim (the sea is still cold at the moment, but some brave souls did go in)While we relax, Antonia and Mixalis cook the fish they have just caught, along with salad, potatoes and their own wine.The food is plentiful, you won't go hungry and delicious.After a leisurely lunch and relax, they then return you to the harbour, with a full stomach and beautiful new made friends.We had such a lovely day with Antonia, Mixalis and the other guests and can not wait to return in September for our third trip.If you are looking for something a little different and also great for kids, give this trip a try.</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>A wonderful day out.</t>
+          <t>Another great day</t>
         </is>
       </c>
       <c r="C45" t="inlineStr"/>
@@ -1173,12 +1173,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Great trip! A bit of a hidden gem as they are a relatively new company operating. Geronimus and Babis are excellent hosts and made us all feel very welcome. It was fascinating watching them pull in their nets from the night before to see what they had caught, and the food they…</t>
+          <t>This was a highlight of our visit to Santorini.  Anthi is so very proud of what she does and her heritage.  It bleeds through in all she does on the fishing trip.  Her crew is very helpful and cheery as well.  We truly enjoyed every minute.  It was very informative to learn about several aspects of fishing from traps to nets to hand lines.  We strongly recommend this fishing experience.</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Fantastic day out</t>
+          <t>An excursion of a lifetime</t>
         </is>
       </c>
       <c r="C46" t="inlineStr"/>
@@ -1189,12 +1189,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>We took the fishing tour with our two children (11 and 13) it was an early start. Antonio very kindly picked us up at 7.40 as we were in Svoronata. The day started with drinks and sailing out to put out the nets and to bring in the nets for the days catch. We couldn’t believe…</t>
+          <t>First of all, Poliegos is the best isle among Milos, Kimolos and Poliegos itself so you must cruise there if you're visiting Kimolos or Milos. It is absolutely one of the best isle in Greece.The cruise is an all day one starting from Pollonia Beach in the morning. We had a stop for a bath at least of 30 minutes in Kato Mersini Beach, Galazia Nera Beach (Blue Bay), another beach in the south coast where we had lunch and finally in another beach in the north coast of Poliegos. He made us to visit some caves along the path too. The captain sailed along the coast trying to make us to see all wonderful water along the coast: he is very expert because he is a fisherman in Milos during the wintertime. We were luckly because the wind, waves, sea and weather so we succedeed to go around completely in Poliegos. We visited also Epano Mersini Beach (Mersine Beach) and Ammoura Beach where is the lighthouse. We had a very long lunch stop where he offered a delicious lunch composed of salads and pasta with fish. It's offering you all drinks for free anytime you would like, not only during the lunch: juices, beer, coke, water and so on.  The captain is VERY kind and funny, the boat is small so there are few tourists on board so the enviroment is very familiar. You can freely ask everything you need at the captain and he'll make the best to satisfy! That money spent with the cruise are the BEST spent of your holiday there! ;) I advice to sail with him because you will not be able to forget easily this "familiar-cruise" because Poliegos and the captain Andreas!</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fantastic Day out ! </t>
+          <t>A "must-sail" cruise around Poliegos</t>
         </is>
       </c>
       <c r="C47" t="inlineStr"/>
@@ -1205,12 +1205,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>This is a boat trip with a difference, a working fishing boat and you watch them haul the nets in...all 2.5km of them! Antonia was the perfect host, answering all our questions, providing us with homemade cake and coffee on arrival, tasty bruschetta later on, then cooking the…</t>
+          <t>It was such a perfect tour including the cake which was prepared for my wife for her birthday. My son loved the fishing and watching them bring in the catch. The food was so well prepared and we even got an octopus which was really good. Can't say enough good things about Anhti and the crew. Ended with a wonderful sunset</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Fantastic day out!</t>
+          <t>Awesome experience and perfect tour</t>
         </is>
       </c>
       <c r="C48" t="inlineStr"/>
@@ -1221,12 +1221,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>We, wife, daughter and I spent a great day out fishing today. On the way to the fishing spots we were given great information on the history of Santorini and then we saw the creels being brought in with shrimp and octopus. Nets were brought in with lots of fish all named by…</t>
+          <t>I can’t say enough about this amazing evening!!! Hands down the best lobster I have ever had in Greece.So, I own a small group of vacation properties on the island. I have always heard amazing reviews of Michali’s Fishing Boat from my guests and decided to give it it a try with a group of friends from the island. I am so happy I did. I highly recommend this to everyone. You will not be disappointed. Andonia and Michalis catered to our every need. Professional courteous and went above and beyond to make our evening cruise memorable. Thank you Andonia and Michalis!</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Great day out fishing</t>
+          <t>Highly Recommend</t>
         </is>
       </c>
       <c r="C49" t="inlineStr"/>
@@ -1237,12 +1237,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Stunning day out with the lovely Efi and Dimitri. Meet the boat at beautiful Kateleios harbour at 8am. Welcome aboard by charming hosts Efi and Dimitri. Motor out to bring in the nets and help as much or as little as you wish to untangle the catch of the day. Swim and Zumba the…</t>
+          <t>We had an amazing time on the boat, there was enough space for all of us and the boat was nice and comfortabele.</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>5*Only way to describe this trip</t>
+          <t>Half a day boat rental</t>
         </is>
       </c>
       <c r="C50" t="inlineStr"/>
@@ -1253,12 +1253,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>We went as a family of 4 having seen the trip on trip advisor before travelling. We were not disappointed. The boat trip lasted around 5-5h 30 and had something for us all...tour around the harbours, fishing, swim in the sea from the boat and then the most amazing bbq of the…</t>
+          <t>This is a must do experience. We recommend it to everyone who wants to swim in crystal blue waters, experience fishing and taste the most delicious fish soup. Frosso and Nikos are very friendly and excellent guests that will amaze you with their hospitality.</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Highly recommend!</t>
+          <t>The best thing we did in Milos!</t>
         </is>
       </c>
       <c r="C51" t="inlineStr"/>
@@ -1269,12 +1269,12 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Since we went in the end of the season, we had the opportunity to go on the fishing trip alone as a couple.  First, the captain navigated us to some places to take nice pictures of the old town of Rhodos. After the photo's we went further on the sea to fish. I'd never fished…</t>
+          <t>Highly recommendable! We had an amazing fishing trip with captain Dimitris! We catched our own fish and even spotted Dolphins! We made an evening trip, we saw a beautiful sunset. Drinks and snacks are on board. Almost every time we dropped in our hook, we catched a fish, unbelievable. Dimistris is a real fisherman, ambitious about fishing and friendly. Thank you for the exciting trip!</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t xml:space="preserve">Great fishing trip! </t>
+          <t>Exciting fishing trip with captain Dimitris!</t>
         </is>
       </c>
       <c r="C52" t="inlineStr"/>
@@ -1285,12 +1285,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>It was such a perfect tour including the cake which was prepared for my wife for her birthday. My son loved the fishing and watching them bring in the catch. The food was so well prepared and we even got an octopus which was really good. Can't say enough good things about Anhti…</t>
+          <t xml:space="preserve">The temperature was awesome, the captain, his wife and his employee were very nice and were always proposing something to drink and to eat. We ate so many kind of fishes and it really worth it. We were only 3 customers on the boat so it was a very private tour. I recommend this activity to everyone!! </t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Awesome experience and perfect tour</t>
+          <t>Very nice day!!</t>
         </is>
       </c>
       <c r="C53" t="inlineStr"/>
@@ -1301,12 +1301,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Absolutely fantastic day! From beginning to end we had a great time. We loved helping get the fish out of the nets, Dimitrios let us be as hands-on as we wanted to. The food cooked and prepared by the couple was delicious and Efi's calamari is THE best around! We even had…</t>
+          <t>My wife and I decided to go on an afternoon fishing trip with Makaroynas Vassilis. Brilliant day out. Antwan and Antonis made every effort possible including a great dinner of fresh fish, salad, bread and dessert. Highly recommend it. H and L</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>This is a must do!</t>
+          <t>Excellent day out</t>
         </is>
       </c>
       <c r="C54" t="inlineStr"/>
@@ -1317,12 +1317,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Efi and Dimitrios are the best hosts you will ever meet. They treat you like family and do everything thing they can to make your fishing experience great. Efi is a great cook.She created a feast which we could not even finish. They obviously love what they do and are happy to…</t>
+          <t>Vassilis and Antonis were absolutely great and gave us an amazing experience. We did not have any experience fishing but still managed to catch a couple small ones due to the very friendly crash course and expertise of the crew! Plenty of time for fishing, and we even made a second stop. To top it up some snorkeling while Vassilis expertly prepares the days catch and some fresh salad and a nice trip back to the harbor!</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Amazing day! Best part of our trip!</t>
+          <t>Perfect Fishing Trip</t>
         </is>
       </c>
       <c r="C55" t="inlineStr"/>
@@ -1333,12 +1333,12 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>I can’t recommend these guys enough! We (2 adults and 2 kids 9y and 11y) went on the Sostis with Captain Stergos. He’s brilliant, patient and great with kids. We had a lovely time and caught lots of fish. Had to throw back a fair few small ones but you can eat the big ones and they will arrange them to be cooked for you after the trip. Thanks!!…</t>
+          <t xml:space="preserve">Just returned from a fantastic day with Efi and Dimitrios. We had a fantastic welcome and I can't recommend highly enough.We wanted to do something a bit different to a standard island cruise and this was perfect. They have a well equipped traditional fishing boat with lots of seating. The first couple of hours were spent reeling their nets in that had been put out the night before and seeing what was caught. Some of this was also a fantastic lunch. Definitely the best meal of our holiday! Also included were drinks and we also had two or three nice long stops for a swim and relax on beaches only accessible by boat.A definite five stars and if we come back to kefalonia again we'll do it again! </t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Fantastic Experience!</t>
+          <t xml:space="preserve">Fantastic day - highly recommended </t>
         </is>
       </c>
       <c r="C56" t="inlineStr"/>
@@ -1349,12 +1349,12 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>We had a fabulous day with Antonia and Michalis on Monday 30 September 2019.    We were picked up by Antonia and taken to the boat early in the morning. When everyone had arrived, there were 11 of us, we were served coffee and homemade cake which was lovely.  We then set sail…</t>
+          <t>My son and I vacationed for a week in Milos and wanted to arrange a guided fishing trip, something we do in most locations we visit. Nikos and his wife agreed to take Ben out even though we knew their season was coming to an end. The weather wasn't great, it rained most of the day. But Nikos and his wife were the most hospitable hosts, so kind and attentive to Ben. He enjoyed catching a snapper and several other fish, they enjoyed a nice lunch together. Ben has not stopped talking about what wonderful people they were. I hope they keep in touch. It was one of the great days of our time in Greece.</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>FISHING TRIP WITH ANTONIA AND MICHALIS ON 30 SEPTEMBER 2019</t>
+          <t>Real fishing in Greece!</t>
         </is>
       </c>
       <c r="C57" t="inlineStr"/>
@@ -1365,12 +1365,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t xml:space="preserve">One of the best experiences in mylos island. We visited kleftiko beach,all the stuff was very kind.Mr Andreas was very helpful and he guide us in the best beaches of the island... </t>
+          <t>A great way to see the islands with your family.  Fresh cooked seafood for lunch caught on your way out to your destination.  It is a must for a first time visit to this island!</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>The best</t>
+          <t>Wonderful way to spend a day on the Aegean Sea!</t>
         </is>
       </c>
       <c r="C58" t="inlineStr"/>
@@ -1381,12 +1381,12 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>The best day my husband and I spent in Milos. Niko, his wife Frossa and the deckhand Simos are awesome people, we felt like part of the family as soon as we put our feet on the boat. Their hospitality is incredible!   We left from the port of Pollonia and visited the islands of…</t>
+          <t>What a great trip. Wonderful value for money, great fun and the best cooked piece of fish all holiday. The Captain (Vasilis?) Is a great, friendly and knowledgeable guy. Loved it! Shaun, Mike and Colin.</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Amazing</t>
+          <t>Boys Fishing Trip</t>
         </is>
       </c>
       <c r="C59" t="inlineStr"/>
@@ -1397,12 +1397,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>We went on an evening fishing trip around 6:30pm - we saw the sunset and dolphins, caught some fish, saw the lunar eclipse and the rest of the amazing night sky. Straight after the trip, which took us to around 10pm, we went to a restaurant where our fresh fish was cooked for us…</t>
+          <t>Very unique experience. Absolutely loved this experience and I am not a person who loves fishing. Just being out on the water and learning about how they use the Nets was interesting. The Captain and crew are awesome. Cooked all the food and everything is top notch. Do this!!</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Must do in Skiathos!</t>
+          <t>Fantastic Experience</t>
         </is>
       </c>
       <c r="C60" t="inlineStr"/>
@@ -1413,12 +1413,12 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>My husband had booked this trip a few weeks before arriving in Kefalonia.   Antonia had contacted us the day before our trip to advise that the weather would not be good (windy) therefore the trip would need to be cancelled.  Although we were disappointed this shows that saftey…</t>
+          <t>Very relaxing day on the water and visited some beautiful spots. The fresh fish was delicous. The crew was very kind and helpful. Would definitely recommend this trip!</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Fantastic Evening!</t>
+          <t>A very nice and relaxing day</t>
         </is>
       </c>
       <c r="C61" t="inlineStr"/>

</xml_diff>